<commit_message>
Adding a Pie Chart to the Montly Cost
</commit_message>
<xml_diff>
--- a/Monthly_Cost_For_FEB_2025.xlsx
+++ b/Monthly_Cost_For_FEB_2025.xlsx
@@ -497,7 +497,7 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>0.0026758182</v>
+        <v>0.0028595836</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -532,7 +532,7 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>1.4096561462</v>
+        <v>1.729895156</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -567,7 +567,7 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>94.68518520160001</v>
+        <v>120.1733963898</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -602,7 +602,7 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>0.273</v>
+        <v>0.3458</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -742,7 +742,7 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>2155.3799044017</v>
+        <v>2635.175254062</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -777,7 +777,7 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>2992.562755</v>
+        <v>3649.560005</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
@@ -812,7 +812,7 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>6.7522</v>
+        <v>8.19</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -847,7 +847,7 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>5.1895733526</v>
+        <v>6.304431389</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -882,7 +882,7 @@
         </is>
       </c>
       <c r="F13" t="n">
-        <v>1300.8078416542</v>
+        <v>1603.4021791513</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
@@ -917,7 +917,7 @@
         </is>
       </c>
       <c r="F14" t="n">
-        <v>118.3785936828</v>
+        <v>154.5104621886</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
@@ -952,7 +952,7 @@
         </is>
       </c>
       <c r="F15" t="n">
-        <v>248.659175137</v>
+        <v>307.0171091574</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -987,7 +987,7 @@
         </is>
       </c>
       <c r="F16" t="n">
-        <v>13.5772</v>
+        <v>16.7804</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -1022,7 +1022,7 @@
         </is>
       </c>
       <c r="F17" t="n">
-        <v>9.619999999999999e-05</v>
+        <v>0.00011908</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
@@ -1057,7 +1057,7 @@
         </is>
       </c>
       <c r="F18" t="n">
-        <v>1.5180208334</v>
+        <v>1.8728125</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
@@ -1127,7 +1127,7 @@
         </is>
       </c>
       <c r="F20" t="n">
-        <v>17.018650869</v>
+        <v>20.9777098817</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
@@ -1162,7 +1162,7 @@
         </is>
       </c>
       <c r="F21" t="n">
-        <v>7.842812978</v>
+        <v>8.8873228444</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
@@ -1197,7 +1197,7 @@
         </is>
       </c>
       <c r="F22" t="n">
-        <v>106.954315448</v>
+        <v>132.2521744562</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
@@ -1232,7 +1232,7 @@
         </is>
       </c>
       <c r="F23" t="n">
-        <v>1.0258864138</v>
+        <v>1.2675174888</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
@@ -1267,7 +1267,7 @@
         </is>
       </c>
       <c r="F24" t="n">
-        <v>0.5075283818</v>
+        <v>0.625927826</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
@@ -1302,7 +1302,7 @@
         </is>
       </c>
       <c r="F25" t="n">
-        <v>0.5146291984</v>
+        <v>0.633047666</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
@@ -1337,7 +1337,7 @@
         </is>
       </c>
       <c r="F26" t="n">
-        <v>41.0621633374</v>
+        <v>50.3766231814</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
@@ -1372,7 +1372,7 @@
         </is>
       </c>
       <c r="F27" t="n">
-        <v>32.623410238</v>
+        <v>40.241514563</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
@@ -1407,7 +1407,7 @@
         </is>
       </c>
       <c r="F28" t="n">
-        <v>0.9127110184</v>
+        <v>1.0305235126</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
@@ -1442,7 +1442,7 @@
         </is>
       </c>
       <c r="F29" t="n">
-        <v>1.0074999504</v>
+        <v>1.2431249388</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
@@ -1477,7 +1477,7 @@
         </is>
       </c>
       <c r="F30" t="n">
-        <v>1.0210218136</v>
+        <v>1.259221192</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
@@ -1512,7 +1512,7 @@
         </is>
       </c>
       <c r="F31" t="n">
-        <v>1266.788482155</v>
+        <v>1525.2493343278</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
@@ -1547,7 +1547,7 @@
         </is>
       </c>
       <c r="F32" t="n">
-        <v>11.5192222654</v>
+        <v>13.8525279433</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
@@ -1617,7 +1617,7 @@
         </is>
       </c>
       <c r="F34" t="n">
-        <v>17.0825873754</v>
+        <v>21.1424751351</v>
       </c>
       <c r="G34" t="inlineStr">
         <is>
@@ -1652,7 +1652,7 @@
         </is>
       </c>
       <c r="F35" t="n">
-        <v>0.9892338109</v>
+        <v>1.2410690078</v>
       </c>
       <c r="G35" t="inlineStr">
         <is>
@@ -1687,7 +1687,7 @@
         </is>
       </c>
       <c r="F36" t="n">
-        <v>2.9693748866</v>
+        <v>3.6747311004</v>
       </c>
       <c r="G36" t="inlineStr">
         <is>
@@ -1722,7 +1722,7 @@
         </is>
       </c>
       <c r="F37" t="n">
-        <v>7.4909585617</v>
+        <v>9.2635173567</v>
       </c>
       <c r="G37" t="inlineStr">
         <is>
@@ -1757,7 +1757,7 @@
         </is>
       </c>
       <c r="F38" t="n">
-        <v>1.4315867349</v>
+        <v>1.7786782584</v>
       </c>
       <c r="G38" t="inlineStr">
         <is>
@@ -1792,7 +1792,7 @@
         </is>
       </c>
       <c r="F39" t="n">
-        <v>7.88689e-05</v>
+        <v>9.90462e-05</v>
       </c>
       <c r="G39" t="inlineStr">
         <is>
@@ -1827,7 +1827,7 @@
         </is>
       </c>
       <c r="F40" t="n">
-        <v>1.3877851092</v>
+        <v>1.7160703202</v>
       </c>
       <c r="G40" t="inlineStr">
         <is>
@@ -1862,7 +1862,7 @@
         </is>
       </c>
       <c r="F41" t="n">
-        <v>81.8993025284</v>
+        <v>99.9634177909</v>
       </c>
       <c r="G41" t="inlineStr">
         <is>
@@ -1897,7 +1897,7 @@
         </is>
       </c>
       <c r="F42" t="n">
-        <v>19.73655775</v>
+        <v>24.34764605</v>
       </c>
       <c r="G42" t="inlineStr">
         <is>
@@ -1932,7 +1932,7 @@
         </is>
       </c>
       <c r="F43" t="n">
-        <v>18.9203014</v>
+        <v>23.398375</v>
       </c>
       <c r="G43" t="inlineStr">
         <is>
@@ -1967,7 +1967,7 @@
         </is>
       </c>
       <c r="F44" t="n">
-        <v>434.7235984</v>
+        <v>496.2506549</v>
       </c>
       <c r="G44" t="inlineStr">
         <is>
@@ -2037,7 +2037,7 @@
         </is>
       </c>
       <c r="F46" t="n">
-        <v>0.0012135711</v>
+        <v>0.0014998431</v>
       </c>
       <c r="G46" t="inlineStr">
         <is>
@@ -2072,7 +2072,7 @@
         </is>
       </c>
       <c r="F47" t="n">
-        <v>30553.2136</v>
+        <v>35600.9745</v>
       </c>
       <c r="G47" t="inlineStr">
         <is>
@@ -2107,7 +2107,7 @@
         </is>
       </c>
       <c r="F48" t="n">
-        <v>0.0712803</v>
+        <v>0.0880971</v>
       </c>
       <c r="G48" t="inlineStr">
         <is>
@@ -2142,7 +2142,7 @@
         </is>
       </c>
       <c r="F49" t="n">
-        <v>102.4460520128</v>
+        <v>126.2575857515</v>
       </c>
       <c r="G49" t="inlineStr">
         <is>
@@ -2177,7 +2177,7 @@
         </is>
       </c>
       <c r="F50" t="n">
-        <v>62.5799347266</v>
+        <v>78.16334437810001</v>
       </c>
       <c r="G50" t="inlineStr">
         <is>
@@ -2212,7 +2212,7 @@
         </is>
       </c>
       <c r="F51" t="n">
-        <v>6.0371055788</v>
+        <v>7.4889260672</v>
       </c>
       <c r="G51" t="inlineStr">
         <is>
@@ -2247,7 +2247,7 @@
         </is>
       </c>
       <c r="F52" t="n">
-        <v>700.5321819016</v>
+        <v>868.1485393352</v>
       </c>
       <c r="G52" t="inlineStr">
         <is>
@@ -2282,7 +2282,7 @@
         </is>
       </c>
       <c r="F53" t="n">
-        <v>22.319646895</v>
+        <v>27.84902393</v>
       </c>
       <c r="G53" t="inlineStr">
         <is>
@@ -2317,7 +2317,7 @@
         </is>
       </c>
       <c r="F54" t="n">
-        <v>49.2006323426</v>
+        <v>60.9658879549</v>
       </c>
       <c r="G54" t="inlineStr">
         <is>
@@ -2352,7 +2352,7 @@
         </is>
       </c>
       <c r="F55" t="n">
-        <v>2.81572655</v>
+        <v>3.4697117</v>
       </c>
       <c r="G55" t="inlineStr">
         <is>
@@ -2387,7 +2387,7 @@
         </is>
       </c>
       <c r="F56" t="n">
-        <v>8206.2400916762</v>
+        <v>10066.6695389534</v>
       </c>
       <c r="G56" t="inlineStr">
         <is>
@@ -2422,7 +2422,7 @@
         </is>
       </c>
       <c r="F57" t="n">
-        <v>0.8313348748</v>
+        <v>1.0899507375</v>
       </c>
       <c r="G57" t="inlineStr">
         <is>
@@ -2457,7 +2457,7 @@
         </is>
       </c>
       <c r="F58" t="n">
-        <v>0.8835005538</v>
+        <v>1.0745591334</v>
       </c>
       <c r="G58" t="inlineStr">
         <is>
@@ -2492,7 +2492,7 @@
         </is>
       </c>
       <c r="F59" t="n">
-        <v>2827.3340900466</v>
+        <v>3473.2365710624</v>
       </c>
       <c r="G59" t="inlineStr">
         <is>
@@ -2527,7 +2527,7 @@
         </is>
       </c>
       <c r="F60" t="n">
-        <v>0.0314577324</v>
+        <v>0.0370797067</v>
       </c>
       <c r="G60" t="inlineStr">
         <is>
@@ -2562,7 +2562,7 @@
         </is>
       </c>
       <c r="F61" t="n">
-        <v>0.0001571037</v>
+        <v>0.0001572051</v>
       </c>
       <c r="G61" t="inlineStr">
         <is>
@@ -2597,7 +2597,7 @@
         </is>
       </c>
       <c r="F62" t="n">
-        <v>80.88535</v>
+        <v>84.44345</v>
       </c>
       <c r="G62" t="inlineStr">
         <is>
@@ -2632,7 +2632,7 @@
         </is>
       </c>
       <c r="F63" t="n">
-        <v>139.5351105466</v>
+        <v>171.2693766866</v>
       </c>
       <c r="G63" t="inlineStr">
         <is>
@@ -2702,7 +2702,7 @@
         </is>
       </c>
       <c r="F65" t="n">
-        <v>0.0801960476</v>
+        <v>0.0986944325</v>
       </c>
       <c r="G65" t="inlineStr">
         <is>
@@ -2737,7 +2737,7 @@
         </is>
       </c>
       <c r="F66" t="n">
-        <v>189.8686892394</v>
+        <v>233.4433500699</v>
       </c>
       <c r="G66" t="inlineStr">
         <is>
@@ -2772,7 +2772,7 @@
         </is>
       </c>
       <c r="F67" t="n">
-        <v>158.7661800722</v>
+        <v>195.1767777946</v>
       </c>
       <c r="G67" t="inlineStr">
         <is>
@@ -2807,7 +2807,7 @@
         </is>
       </c>
       <c r="F68" t="n">
-        <v>50.823140527</v>
+        <v>68.041742654</v>
       </c>
       <c r="G68" t="inlineStr">
         <is>
@@ -2842,7 +2842,7 @@
         </is>
       </c>
       <c r="F69" t="n">
-        <v>1.059968</v>
+        <v>1.424332</v>
       </c>
       <c r="G69" t="inlineStr">
         <is>
@@ -2877,7 +2877,7 @@
         </is>
       </c>
       <c r="F70" t="n">
-        <v>26.2041144542</v>
+        <v>28.3215987377</v>
       </c>
       <c r="G70" t="inlineStr">
         <is>
@@ -2912,7 +2912,7 @@
         </is>
       </c>
       <c r="F71" t="n">
-        <v>57.9921862595</v>
+        <v>71.5660516225</v>
       </c>
       <c r="G71" t="inlineStr">
         <is>
@@ -2947,7 +2947,7 @@
         </is>
       </c>
       <c r="F72" t="n">
-        <v>1.0558275365</v>
+        <v>1.4201915535</v>
       </c>
       <c r="G72" t="inlineStr">
         <is>
@@ -2982,7 +2982,7 @@
         </is>
       </c>
       <c r="F73" t="n">
-        <v>92.562163614</v>
+        <v>114.1935810958</v>
       </c>
       <c r="G73" t="inlineStr">
         <is>
@@ -3017,7 +3017,7 @@
         </is>
       </c>
       <c r="F74" t="n">
-        <v>0.0185407882</v>
+        <v>0.0228537523</v>
       </c>
       <c r="G74" t="inlineStr">
         <is>
@@ -3052,7 +3052,7 @@
         </is>
       </c>
       <c r="F75" t="n">
-        <v>0.05638611</v>
+        <v>0.06950266500000001</v>
       </c>
       <c r="G75" t="inlineStr">
         <is>
@@ -3087,7 +3087,7 @@
         </is>
       </c>
       <c r="F76" t="n">
-        <v>0.2030749723</v>
+        <v>0.2509693034</v>
       </c>
       <c r="G76" t="inlineStr">
         <is>
@@ -3122,7 +3122,7 @@
         </is>
       </c>
       <c r="F77" t="n">
-        <v>420.2260706159</v>
+        <v>517.8209328546</v>
       </c>
       <c r="G77" t="inlineStr">
         <is>
@@ -3157,7 +3157,7 @@
         </is>
       </c>
       <c r="F78" t="n">
-        <v>10441.4637687853</v>
+        <v>12066.6509785139</v>
       </c>
       <c r="G78" t="inlineStr">
         <is>
@@ -3192,7 +3192,7 @@
         </is>
       </c>
       <c r="F79" t="n">
-        <v>149.06892</v>
+        <v>182.94822</v>
       </c>
       <c r="G79" t="inlineStr">
         <is>
@@ -3227,7 +3227,7 @@
         </is>
       </c>
       <c r="F80" t="n">
-        <v>3914.04741</v>
+        <v>4649.54854</v>
       </c>
       <c r="G80" t="inlineStr">
         <is>
@@ -3297,7 +3297,7 @@
         </is>
       </c>
       <c r="F82" t="n">
-        <v>2539.55429</v>
+        <v>3147.53439</v>
       </c>
       <c r="G82" t="inlineStr">
         <is>
@@ -3332,7 +3332,7 @@
         </is>
       </c>
       <c r="F83" t="n">
-        <v>222.88812</v>
+        <v>256.76742</v>
       </c>
       <c r="G83" t="inlineStr">
         <is>
@@ -3367,7 +3367,7 @@
         </is>
       </c>
       <c r="F84" t="n">
-        <v>18203.6578151943</v>
+        <v>22078.0617196826</v>
       </c>
       <c r="G84" t="inlineStr">
         <is>
@@ -3402,7 +3402,7 @@
         </is>
       </c>
       <c r="F85" t="n">
-        <v>0.3975833211</v>
+        <v>0.4907499849</v>
       </c>
       <c r="G85" t="inlineStr">
         <is>
@@ -3437,7 +3437,7 @@
         </is>
       </c>
       <c r="F86" t="n">
-        <v>15.3153028536</v>
+        <v>18.8779537433</v>
       </c>
       <c r="G86" t="inlineStr">
         <is>
@@ -3472,7 +3472,7 @@
         </is>
       </c>
       <c r="F87" t="n">
-        <v>552.3984390982999</v>
+        <v>707.2294144587</v>
       </c>
       <c r="G87" t="inlineStr">
         <is>
@@ -3507,7 +3507,7 @@
         </is>
       </c>
       <c r="F88" t="n">
-        <v>0.3975833211</v>
+        <v>0.4907499849</v>
       </c>
       <c r="G88" t="inlineStr">
         <is>
@@ -3542,7 +3542,7 @@
         </is>
       </c>
       <c r="F89" t="n">
-        <v>9.939583321100001</v>
+        <v>12.2687499849</v>
       </c>
       <c r="G89" t="inlineStr">
         <is>
@@ -3577,7 +3577,7 @@
         </is>
       </c>
       <c r="F90" t="n">
-        <v>742.1974431684999</v>
+        <v>912.8759326054</v>
       </c>
       <c r="G90" t="inlineStr">
         <is>
@@ -3612,7 +3612,7 @@
         </is>
       </c>
       <c r="F91" t="n">
-        <v>10.9380137515</v>
+        <v>13.234859925</v>
       </c>
       <c r="G91" t="inlineStr">
         <is>
@@ -3647,7 +3647,7 @@
         </is>
       </c>
       <c r="F92" t="n">
-        <v>3377.0845870113</v>
+        <v>4172.1726677679</v>
       </c>
       <c r="G92" t="inlineStr">
         <is>
@@ -3682,7 +3682,7 @@
         </is>
       </c>
       <c r="F93" t="n">
-        <v>299.8972673839</v>
+        <v>343.2200002973</v>
       </c>
       <c r="G93" t="inlineStr">
         <is>
@@ -3717,7 +3717,7 @@
         </is>
       </c>
       <c r="F94" t="n">
-        <v>17374.9539908915</v>
+        <v>21355.5253412426</v>
       </c>
       <c r="G94" t="inlineStr">
         <is>
@@ -3752,7 +3752,7 @@
         </is>
       </c>
       <c r="F95" t="n">
-        <v>1.5776e-06</v>
+        <v>2.109e-06</v>
       </c>
       <c r="G95" t="inlineStr">
         <is>
@@ -3787,7 +3787,7 @@
         </is>
       </c>
       <c r="F96" t="n">
-        <v>263.7284487072</v>
+        <v>323.6956409823</v>
       </c>
       <c r="G96" t="inlineStr">
         <is>
@@ -3822,7 +3822,7 @@
         </is>
       </c>
       <c r="F97" t="n">
-        <v>130.34112</v>
+        <v>160.7424</v>
       </c>
       <c r="G97" t="inlineStr">
         <is>
@@ -3857,7 +3857,7 @@
         </is>
       </c>
       <c r="F98" t="n">
-        <v>3940.0589359393</v>
+        <v>4864.6088185825</v>
       </c>
       <c r="G98" t="inlineStr">
         <is>
@@ -3892,7 +3892,7 @@
         </is>
       </c>
       <c r="F99" t="n">
-        <v>568.2068876261</v>
+        <v>756.2233465401</v>
       </c>
       <c r="G99" t="inlineStr">
         <is>
@@ -3927,7 +3927,7 @@
         </is>
       </c>
       <c r="F100" t="n">
-        <v>43603.4427243323</v>
+        <v>53250.015698637</v>
       </c>
       <c r="G100" t="inlineStr">
         <is>
@@ -3962,7 +3962,7 @@
         </is>
       </c>
       <c r="F101" t="n">
-        <v>256.6654471341</v>
+        <v>312.2180085215</v>
       </c>
       <c r="G101" t="inlineStr">
         <is>
@@ -3997,7 +3997,7 @@
         </is>
       </c>
       <c r="F102" t="n">
-        <v>4682.0188211189</v>
+        <v>5714.1329628324</v>
       </c>
       <c r="G102" t="inlineStr">
         <is>
@@ -4032,7 +4032,7 @@
         </is>
       </c>
       <c r="F103" t="n">
-        <v>463.7406428948</v>
+        <v>572.4725372717</v>
       </c>
       <c r="G103" t="inlineStr">
         <is>
@@ -4067,7 +4067,7 @@
         </is>
       </c>
       <c r="F104" t="n">
-        <v>295.2876266741</v>
+        <v>366.6316266741</v>
       </c>
       <c r="G104" t="inlineStr">
         <is>
@@ -4102,7 +4102,7 @@
         </is>
       </c>
       <c r="F105" t="n">
-        <v>305.942</v>
+        <v>377.559</v>
       </c>
       <c r="G105" t="inlineStr">
         <is>
@@ -4137,7 +4137,7 @@
         </is>
       </c>
       <c r="F106" t="n">
-        <v>827.8213436463</v>
+        <v>852.0738010447</v>
       </c>
       <c r="G106" t="inlineStr">
         <is>
@@ -4277,7 +4277,7 @@
         </is>
       </c>
       <c r="F110" t="n">
-        <v>4228.0014657707</v>
+        <v>5208.8544333595</v>
       </c>
       <c r="G110" t="inlineStr">
         <is>
@@ -4312,7 +4312,7 @@
         </is>
       </c>
       <c r="F111" t="n">
-        <v>7.6583131582</v>
+        <v>9.4397587632</v>
       </c>
       <c r="G111" t="inlineStr">
         <is>
@@ -4347,7 +4347,7 @@
         </is>
       </c>
       <c r="F112" t="n">
-        <v>11.4187422017</v>
+        <v>13.9495974567</v>
       </c>
       <c r="G112" t="inlineStr">
         <is>
@@ -4382,7 +4382,7 @@
         </is>
       </c>
       <c r="F113" t="n">
-        <v>38.3795092557</v>
+        <v>47.3195803431</v>
       </c>
       <c r="G113" t="inlineStr">
         <is>
@@ -4417,7 +4417,7 @@
         </is>
       </c>
       <c r="F114" t="n">
-        <v>128.8774698795</v>
+        <v>160.678752495</v>
       </c>
       <c r="G114" t="inlineStr">
         <is>
@@ -4452,7 +4452,7 @@
         </is>
       </c>
       <c r="F115" t="n">
-        <v>44.4563508928</v>
+        <v>53.4203274625</v>
       </c>
       <c r="G115" t="inlineStr">
         <is>
@@ -4487,7 +4487,7 @@
         </is>
       </c>
       <c r="F116" t="n">
-        <v>1066.642704324</v>
+        <v>1314.0229964301</v>
       </c>
       <c r="G116" t="inlineStr">
         <is>
@@ -4522,7 +4522,7 @@
         </is>
       </c>
       <c r="F117" t="n">
-        <v>7.65765</v>
+        <v>9.438974999999999</v>
       </c>
       <c r="G117" t="inlineStr">
         <is>
@@ -4557,7 +4557,7 @@
         </is>
       </c>
       <c r="F118" t="n">
-        <v>8.596531516800001</v>
+        <v>10.5926806058</v>
       </c>
       <c r="G118" t="inlineStr">
         <is>
@@ -4592,7 +4592,7 @@
         </is>
       </c>
       <c r="F119" t="n">
-        <v>52.1091535528</v>
+        <v>62.8841987549</v>
       </c>
       <c r="G119" t="inlineStr">
         <is>
@@ -4627,7 +4627,7 @@
         </is>
       </c>
       <c r="F120" t="n">
-        <v>1.2581314602</v>
+        <v>1.593632331</v>
       </c>
       <c r="G120" t="inlineStr">
         <is>
@@ -4662,7 +4662,7 @@
         </is>
       </c>
       <c r="F121" t="n">
-        <v>2243.9193347229</v>
+        <v>2675.6432846923</v>
       </c>
       <c r="G121" t="inlineStr">
         <is>
@@ -4732,7 +4732,7 @@
         </is>
       </c>
       <c r="F123" t="n">
-        <v>61.4276554327</v>
+        <v>75.69373774739999</v>
       </c>
       <c r="G123" t="inlineStr">
         <is>
@@ -4767,7 +4767,7 @@
         </is>
       </c>
       <c r="F124" t="n">
-        <v>8.9745392789</v>
+        <v>11.1952990434</v>
       </c>
       <c r="G124" t="inlineStr">
         <is>
@@ -4802,7 +4802,7 @@
         </is>
       </c>
       <c r="F125" t="n">
-        <v>4.6946834639</v>
+        <v>5.7901784147</v>
       </c>
       <c r="G125" t="inlineStr">
         <is>
@@ -4837,7 +4837,7 @@
         </is>
       </c>
       <c r="F126" t="n">
-        <v>0.000752115</v>
+        <v>0.00088816</v>
       </c>
       <c r="G126" t="inlineStr">
         <is>
@@ -4872,7 +4872,7 @@
         </is>
       </c>
       <c r="F127" t="n">
-        <v>30.6488625961</v>
+        <v>37.7840855443</v>
       </c>
       <c r="G127" t="inlineStr">
         <is>
@@ -4907,7 +4907,7 @@
         </is>
       </c>
       <c r="F128" t="n">
-        <v>108.3349200807</v>
+        <v>133.9115030289</v>
       </c>
       <c r="G128" t="inlineStr">
         <is>
@@ -4942,7 +4942,7 @@
         </is>
       </c>
       <c r="F129" t="n">
-        <v>107.8141110049</v>
+        <v>133.2502781539</v>
       </c>
       <c r="G129" t="inlineStr">
         <is>
@@ -4977,7 +4977,7 @@
         </is>
       </c>
       <c r="F130" t="n">
-        <v>1.12203</v>
+        <v>1.421238</v>
       </c>
       <c r="G130" t="inlineStr">
         <is>
@@ -5082,7 +5082,7 @@
         </is>
       </c>
       <c r="F133" t="n">
-        <v>67.5479551226</v>
+        <v>83.2609673489</v>
       </c>
       <c r="G133" t="inlineStr">
         <is>
@@ -5117,7 +5117,7 @@
         </is>
       </c>
       <c r="F134" t="n">
-        <v>94.33252400000001</v>
+        <v>116.276186</v>
       </c>
       <c r="G134" t="inlineStr">
         <is>
@@ -5152,7 +5152,7 @@
         </is>
       </c>
       <c r="F135" t="n">
-        <v>3510.6197598752</v>
+        <v>4485.8566436044</v>
       </c>
       <c r="G135" t="inlineStr">
         <is>
@@ -5187,7 +5187,7 @@
         </is>
       </c>
       <c r="F136" t="n">
-        <v>834.6057935374999</v>
+        <v>1147.4491423515</v>
       </c>
       <c r="G136" t="inlineStr">
         <is>
@@ -5222,7 +5222,7 @@
         </is>
       </c>
       <c r="F137" t="n">
-        <v>1346.53665548</v>
+        <v>1660.04985548</v>
       </c>
       <c r="G137" t="inlineStr">
         <is>
@@ -5257,7 +5257,7 @@
         </is>
       </c>
       <c r="F138" t="n">
-        <v>2.4260378815</v>
+        <v>2.9597507463</v>
       </c>
       <c r="G138" t="inlineStr">
         <is>
@@ -5292,7 +5292,7 @@
         </is>
       </c>
       <c r="F139" t="n">
-        <v>1043.5717911453</v>
+        <v>1286.3331333505</v>
       </c>
       <c r="G139" t="inlineStr">
         <is>
@@ -5327,7 +5327,7 @@
         </is>
       </c>
       <c r="F140" t="n">
-        <v>5881.7865097296</v>
+        <v>7189.9062170882</v>
       </c>
       <c r="G140" t="inlineStr">
         <is>
@@ -5362,7 +5362,7 @@
         </is>
       </c>
       <c r="F141" t="n">
-        <v>17271.9841733144</v>
+        <v>21281.5932880336</v>
       </c>
       <c r="G141" t="inlineStr">
         <is>
@@ -5397,7 +5397,7 @@
         </is>
       </c>
       <c r="F142" t="n">
-        <v>57.9026580785</v>
+        <v>71.3720864754</v>
       </c>
       <c r="G142" t="inlineStr">
         <is>
@@ -5432,7 +5432,7 @@
         </is>
       </c>
       <c r="F143" t="n">
-        <v>1124.6974703674</v>
+        <v>1379.1889799141</v>
       </c>
       <c r="G143" t="inlineStr">
         <is>
@@ -5467,7 +5467,7 @@
         </is>
       </c>
       <c r="F144" t="n">
-        <v>18.4731634548</v>
+        <v>22.8571359778</v>
       </c>
       <c r="G144" t="inlineStr">
         <is>
@@ -5502,7 +5502,7 @@
         </is>
       </c>
       <c r="F145" t="n">
-        <v>726.8869798429999</v>
+        <v>771.9926668418</v>
       </c>
       <c r="G145" t="inlineStr">
         <is>
@@ -5572,7 +5572,7 @@
         </is>
       </c>
       <c r="F147" t="n">
-        <v>45520.551973349</v>
+        <v>53177.084449512</v>
       </c>
       <c r="G147" t="inlineStr">
         <is>
@@ -5607,7 +5607,7 @@
         </is>
       </c>
       <c r="F148" t="n">
-        <v>0.0008747969</v>
+        <v>0.0010741474</v>
       </c>
       <c r="G148" t="inlineStr">
         <is>
@@ -5642,7 +5642,7 @@
         </is>
       </c>
       <c r="F149" t="n">
-        <v>1639.352671572</v>
+        <v>1914.9600314418</v>
       </c>
       <c r="G149" t="inlineStr">
         <is>
@@ -5677,7 +5677,7 @@
         </is>
       </c>
       <c r="F150" t="n">
-        <v>85.04731527200001</v>
+        <v>86.787900146</v>
       </c>
       <c r="G150" t="inlineStr">
         <is>
@@ -5712,7 +5712,7 @@
         </is>
       </c>
       <c r="F151" t="n">
-        <v>7772.5014241688</v>
+        <v>9347.2149325635</v>
       </c>
       <c r="G151" t="inlineStr">
         <is>
@@ -5747,7 +5747,7 @@
         </is>
       </c>
       <c r="F152" t="n">
-        <v>125.417128921</v>
+        <v>148.5581334661</v>
       </c>
       <c r="G152" t="inlineStr">
         <is>
@@ -5782,7 +5782,7 @@
         </is>
       </c>
       <c r="F153" t="n">
-        <v>943.7810412661</v>
+        <v>1104.0924220489</v>
       </c>
       <c r="G153" t="inlineStr">
         <is>
@@ -5817,7 +5817,7 @@
         </is>
       </c>
       <c r="F154" t="n">
-        <v>0.149342284</v>
+        <v>0.157312246</v>
       </c>
       <c r="G154" t="inlineStr">
         <is>
@@ -5957,7 +5957,7 @@
         </is>
       </c>
       <c r="F158" t="n">
-        <v>0.455086632</v>
+        <v>0.455097552</v>
       </c>
       <c r="G158" t="inlineStr">
         <is>
@@ -5992,7 +5992,7 @@
         </is>
       </c>
       <c r="F159" t="n">
-        <v>11.103447082</v>
+        <v>11.546665858</v>
       </c>
       <c r="G159" t="inlineStr">
         <is>
@@ -6027,7 +6027,7 @@
         </is>
       </c>
       <c r="F160" t="n">
-        <v>10.709539568</v>
+        <v>11.846281902</v>
       </c>
       <c r="G160" t="inlineStr">
         <is>
@@ -6062,7 +6062,7 @@
         </is>
       </c>
       <c r="F161" t="n">
-        <v>0.091064064</v>
+        <v>0.09107225400000001</v>
       </c>
       <c r="G161" t="inlineStr">
         <is>
@@ -6097,7 +6097,7 @@
         </is>
       </c>
       <c r="F162" t="n">
-        <v>0.091019656</v>
+        <v>0.091022204</v>
       </c>
       <c r="G162" t="inlineStr">
         <is>
@@ -6167,7 +6167,7 @@
         </is>
       </c>
       <c r="F164" t="n">
-        <v>2129.8368300002</v>
+        <v>2626.989432189</v>
       </c>
       <c r="G164" t="inlineStr">
         <is>
@@ -6202,7 +6202,7 @@
         </is>
       </c>
       <c r="F165" t="n">
-        <v>7.8339891673</v>
+        <v>9.128752221699999</v>
       </c>
       <c r="G165" t="inlineStr">
         <is>
@@ -6237,7 +6237,7 @@
         </is>
       </c>
       <c r="F166" t="n">
-        <v>12.8918507671</v>
+        <v>16.0037708058</v>
       </c>
       <c r="G166" t="inlineStr">
         <is>
@@ -6272,7 +6272,7 @@
         </is>
       </c>
       <c r="F167" t="n">
-        <v>0.0030986237</v>
+        <v>0.0038460557</v>
       </c>
       <c r="G167" t="inlineStr">
         <is>
@@ -6307,7 +6307,7 @@
         </is>
       </c>
       <c r="F168" t="n">
-        <v>5.46e-05</v>
+        <v>6.916e-05</v>
       </c>
       <c r="G168" t="inlineStr">
         <is>
@@ -6342,7 +6342,7 @@
         </is>
       </c>
       <c r="F169" t="n">
-        <v>0.000536445</v>
+        <v>0.000662025</v>
       </c>
       <c r="G169" t="inlineStr">
         <is>
@@ -6377,7 +6377,7 @@
         </is>
       </c>
       <c r="F170" t="n">
-        <v>2.7755e-05</v>
+        <v>3.5035e-05</v>
       </c>
       <c r="G170" t="inlineStr">
         <is>
@@ -6412,7 +6412,7 @@
         </is>
       </c>
       <c r="F171" t="n">
-        <v>19.8348716831</v>
+        <v>24.590330339</v>
       </c>
       <c r="G171" t="inlineStr">
         <is>
@@ -6447,7 +6447,7 @@
         </is>
       </c>
       <c r="F172" t="n">
-        <v>6.006e-05</v>
+        <v>7.462e-05</v>
       </c>
       <c r="G172" t="inlineStr">
         <is>
@@ -6482,7 +6482,7 @@
         </is>
       </c>
       <c r="F173" t="n">
-        <v>0.5306309953</v>
+        <v>0.6547884094999999</v>
       </c>
       <c r="G173" t="inlineStr">
         <is>
@@ -6517,7 +6517,7 @@
         </is>
       </c>
       <c r="F174" t="n">
-        <v>0.7324131455</v>
+        <v>0.9047634666</v>
       </c>
       <c r="G174" t="inlineStr">
         <is>
@@ -6552,7 +6552,7 @@
         </is>
       </c>
       <c r="F175" t="n">
-        <v>23834.5709585269</v>
+        <v>29397.8149025704</v>
       </c>
       <c r="G175" t="inlineStr">
         <is>
@@ -6587,7 +6587,7 @@
         </is>
       </c>
       <c r="F176" t="n">
-        <v>0.0342160672</v>
+        <v>0.0442590753</v>
       </c>
       <c r="G176" t="inlineStr">
         <is>
@@ -6622,7 +6622,7 @@
         </is>
       </c>
       <c r="F177" t="n">
-        <v>0.0004291028</v>
+        <v>0.0005246881</v>
       </c>
       <c r="G177" t="inlineStr">
         <is>
@@ -6657,7 +6657,7 @@
         </is>
       </c>
       <c r="F178" t="n">
-        <v>0.0407315276</v>
+        <v>0.0512264277</v>
       </c>
       <c r="G178" t="inlineStr">
         <is>
@@ -6692,7 +6692,7 @@
         </is>
       </c>
       <c r="F179" t="n">
-        <v>5.004221107</v>
+        <v>5.930493209</v>
       </c>
       <c r="G179" t="inlineStr">
         <is>
@@ -6727,7 +6727,7 @@
         </is>
       </c>
       <c r="F180" t="n">
-        <v>0.0004657578</v>
+        <v>0.0005747077</v>
       </c>
       <c r="G180" t="inlineStr">
         <is>
@@ -6762,7 +6762,7 @@
         </is>
       </c>
       <c r="F181" t="n">
-        <v>0.0013180666</v>
+        <v>0.0016330453</v>
       </c>
       <c r="G181" t="inlineStr">
         <is>
@@ -6797,7 +6797,7 @@
         </is>
       </c>
       <c r="F182" t="n">
-        <v>11.1829522</v>
+        <v>14.0911359525</v>
       </c>
       <c r="G182" t="inlineStr">
         <is>
@@ -6832,7 +6832,7 @@
         </is>
       </c>
       <c r="F183" t="n">
-        <v>0.0446443991</v>
+        <v>0.0567836938</v>
       </c>
       <c r="G183" t="inlineStr">
         <is>
@@ -6867,7 +6867,7 @@
         </is>
       </c>
       <c r="F184" t="n">
-        <v>1199.9577788963</v>
+        <v>1411.4715951225</v>
       </c>
       <c r="G184" t="inlineStr">
         <is>
@@ -6902,7 +6902,7 @@
         </is>
       </c>
       <c r="F185" t="n">
-        <v>1.3793271349</v>
+        <v>1.7899800062</v>
       </c>
       <c r="G185" t="inlineStr">
         <is>
@@ -6937,7 +6937,7 @@
         </is>
       </c>
       <c r="F186" t="n">
-        <v>8763.274011445001</v>
+        <v>11073.5401686086</v>
       </c>
       <c r="G186" t="inlineStr">
         <is>
@@ -6972,7 +6972,7 @@
         </is>
       </c>
       <c r="F187" t="n">
-        <v>0.0004744612</v>
+        <v>0.0005881497</v>
       </c>
       <c r="G187" t="inlineStr">
         <is>
@@ -7007,7 +7007,7 @@
         </is>
       </c>
       <c r="F188" t="n">
-        <v>0.002879019</v>
+        <v>0.0032658275</v>
       </c>
       <c r="G188" t="inlineStr">
         <is>
@@ -7042,7 +7042,7 @@
         </is>
       </c>
       <c r="F189" t="n">
-        <v>5.632e-07</v>
+        <v>6.855e-07</v>
       </c>
       <c r="G189" t="inlineStr">
         <is>
@@ -7077,7 +7077,7 @@
         </is>
       </c>
       <c r="F190" t="n">
-        <v>6.624e-06</v>
+        <v>8.073e-06</v>
       </c>
       <c r="G190" t="inlineStr">
         <is>
@@ -7112,7 +7112,7 @@
         </is>
       </c>
       <c r="F191" t="n">
-        <v>6266.0205669912</v>
+        <v>7573.0797291726</v>
       </c>
       <c r="G191" t="inlineStr">
         <is>
@@ -7147,7 +7147,7 @@
         </is>
       </c>
       <c r="F192" t="n">
-        <v>1.7017</v>
+        <v>2.09755</v>
       </c>
       <c r="G192" t="inlineStr">
         <is>
@@ -7182,7 +7182,7 @@
         </is>
       </c>
       <c r="F193" t="n">
-        <v>50.9782</v>
+        <v>62.972</v>
       </c>
       <c r="G193" t="inlineStr">
         <is>
@@ -7217,7 +7217,7 @@
         </is>
       </c>
       <c r="F194" t="n">
-        <v>1.7017</v>
+        <v>2.09755</v>
       </c>
       <c r="G194" t="inlineStr">
         <is>
@@ -7252,7 +7252,7 @@
         </is>
       </c>
       <c r="F195" t="n">
-        <v>72.9688310901</v>
+        <v>90.1814938591</v>
       </c>
       <c r="G195" t="inlineStr">
         <is>
@@ -7287,7 +7287,7 @@
         </is>
       </c>
       <c r="F196" t="n">
-        <v>46.0687002132</v>
+        <v>56.9613993298</v>
       </c>
       <c r="G196" t="inlineStr">
         <is>
@@ -7322,7 +7322,7 @@
         </is>
       </c>
       <c r="F197" t="n">
-        <v>3.38975</v>
+        <v>4.18145</v>
       </c>
       <c r="G197" t="inlineStr">
         <is>
@@ -7392,7 +7392,7 @@
         </is>
       </c>
       <c r="F199" t="n">
-        <v>8093.7511180527</v>
+        <v>9703.735095814</v>
       </c>
       <c r="G199" t="inlineStr">
         <is>
@@ -7427,7 +7427,7 @@
         </is>
       </c>
       <c r="F200" t="n">
-        <v>1.1903125</v>
+        <v>1.43771875</v>
       </c>
       <c r="G200" t="inlineStr">
         <is>
@@ -7462,7 +7462,7 @@
         </is>
       </c>
       <c r="F201" t="n">
-        <v>1.20575</v>
+        <v>1.4885</v>
       </c>
       <c r="G201" t="inlineStr">
         <is>
@@ -7497,7 +7497,7 @@
         </is>
       </c>
       <c r="F202" t="n">
-        <v>462.5068174499</v>
+        <v>572.8042982898</v>
       </c>
       <c r="G202" t="inlineStr">
         <is>
@@ -7532,7 +7532,7 @@
         </is>
       </c>
       <c r="F203" t="n">
-        <v>2095.1261106389</v>
+        <v>2591.1368593169</v>
       </c>
       <c r="G203" t="inlineStr">
         <is>
@@ -7567,7 +7567,7 @@
         </is>
       </c>
       <c r="F204" t="n">
-        <v>99.00041656720001</v>
+        <v>122.3570832104</v>
       </c>
       <c r="G204" t="inlineStr">
         <is>
@@ -7637,7 +7637,7 @@
         </is>
       </c>
       <c r="F206" t="n">
-        <v>1.3313347961</v>
+        <v>1.5568427774</v>
       </c>
       <c r="G206" t="inlineStr">
         <is>
@@ -7707,7 +7707,7 @@
         </is>
       </c>
       <c r="F208" t="n">
-        <v>5994.76</v>
+        <v>7193.53</v>
       </c>
       <c r="G208" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Adjustin For End Of February Data
</commit_message>
<xml_diff>
--- a/Monthly_Cost_For_FEB_2025.xlsx
+++ b/Monthly_Cost_For_FEB_2025.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G209"/>
+  <dimension ref="A1:G211"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -497,7 +497,7 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>0.0028595836</v>
+        <v>0.0029738842</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -532,7 +532,7 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>1.729895156</v>
+        <v>2.5949120566</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -567,7 +567,7 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>120.1733963898</v>
+        <v>177.633760284</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -602,7 +602,7 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>0.3458</v>
+        <v>0.5096000000000001</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -742,7 +742,7 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>2635.175254062</v>
+        <v>3747.2518104489</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -777,7 +777,7 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>3649.560005</v>
+        <v>4374.66666</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
@@ -812,7 +812,7 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>8.19</v>
+        <v>10.647</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -847,7 +847,7 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>6.304431389</v>
+        <v>9.851032035599999</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -882,7 +882,7 @@
         </is>
       </c>
       <c r="F13" t="n">
-        <v>1603.4021791513</v>
+        <v>2337.2803999776</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
@@ -917,7 +917,7 @@
         </is>
       </c>
       <c r="F14" t="n">
-        <v>154.5104621886</v>
+        <v>242.140626036</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
@@ -952,7 +952,7 @@
         </is>
       </c>
       <c r="F15" t="n">
-        <v>307.0171091574</v>
+        <v>447.2365646398</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -987,7 +987,7 @@
         </is>
       </c>
       <c r="F16" t="n">
-        <v>16.7804</v>
+        <v>24.4608</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -1022,7 +1022,7 @@
         </is>
       </c>
       <c r="F17" t="n">
-        <v>0.00011908</v>
+        <v>0.00017472</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
@@ -1057,7 +1057,7 @@
         </is>
       </c>
       <c r="F18" t="n">
-        <v>1.8728125</v>
+        <v>2.73</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
@@ -1127,7 +1127,7 @@
         </is>
       </c>
       <c r="F20" t="n">
-        <v>20.9777098817</v>
+        <v>30.5792963175</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
@@ -1162,7 +1162,7 @@
         </is>
       </c>
       <c r="F21" t="n">
-        <v>8.8873228444</v>
+        <v>9.334546421200001</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
@@ -1197,7 +1197,7 @@
         </is>
       </c>
       <c r="F22" t="n">
-        <v>132.2521744562</v>
+        <v>191.7641459624</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
@@ -1232,7 +1232,7 @@
         </is>
       </c>
       <c r="F23" t="n">
-        <v>1.2675174888</v>
+        <v>1.8557219604</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
@@ -1267,7 +1267,7 @@
         </is>
       </c>
       <c r="F24" t="n">
-        <v>0.625927826</v>
+        <v>0.9134069952</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
@@ -1302,7 +1302,7 @@
         </is>
       </c>
       <c r="F25" t="n">
-        <v>0.633047666</v>
+        <v>0.9207479652</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
@@ -1337,7 +1337,7 @@
         </is>
       </c>
       <c r="F26" t="n">
-        <v>50.3766231814</v>
+        <v>72.9550952554</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
@@ -1372,7 +1372,7 @@
         </is>
       </c>
       <c r="F27" t="n">
-        <v>40.241514563</v>
+        <v>58.864917249</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
@@ -1407,7 +1407,7 @@
         </is>
       </c>
       <c r="F28" t="n">
-        <v>1.0305235126</v>
+        <v>1.3176068318</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
@@ -1442,7 +1442,7 @@
         </is>
       </c>
       <c r="F29" t="n">
-        <v>1.2431249388</v>
+        <v>1.8172915772</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
@@ -1477,7 +1477,7 @@
         </is>
       </c>
       <c r="F30" t="n">
-        <v>1.259221192</v>
+        <v>1.8344989404</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
@@ -1512,7 +1512,7 @@
         </is>
       </c>
       <c r="F31" t="n">
-        <v>1525.2493343278</v>
+        <v>2109.5480974192</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
@@ -1547,7 +1547,7 @@
         </is>
       </c>
       <c r="F32" t="n">
-        <v>13.8525279433</v>
+        <v>21.2085005003</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
@@ -1617,7 +1617,7 @@
         </is>
       </c>
       <c r="F34" t="n">
-        <v>21.1424751351</v>
+        <v>28.6582294279</v>
       </c>
       <c r="G34" t="inlineStr">
         <is>
@@ -1652,7 +1652,7 @@
         </is>
       </c>
       <c r="F35" t="n">
-        <v>1.2410690078</v>
+        <v>1.8695488864</v>
       </c>
       <c r="G35" t="inlineStr">
         <is>
@@ -1687,7 +1687,7 @@
         </is>
       </c>
       <c r="F36" t="n">
-        <v>3.6747311004</v>
+        <v>5.3523101125</v>
       </c>
       <c r="G36" t="inlineStr">
         <is>
@@ -1722,7 +1722,7 @@
         </is>
       </c>
       <c r="F37" t="n">
-        <v>9.2635173567</v>
+        <v>13.5220707548</v>
       </c>
       <c r="G37" t="inlineStr">
         <is>
@@ -1757,7 +1757,7 @@
         </is>
       </c>
       <c r="F38" t="n">
-        <v>1.7786782584</v>
+        <v>2.3794293929</v>
       </c>
       <c r="G38" t="inlineStr">
         <is>
@@ -1792,7 +1792,7 @@
         </is>
       </c>
       <c r="F39" t="n">
-        <v>9.90462e-05</v>
+        <v>0.0001303275</v>
       </c>
       <c r="G39" t="inlineStr">
         <is>
@@ -1827,7 +1827,7 @@
         </is>
       </c>
       <c r="F40" t="n">
-        <v>1.7160703202</v>
+        <v>1.8485938303</v>
       </c>
       <c r="G40" t="inlineStr">
         <is>
@@ -1862,7 +1862,7 @@
         </is>
       </c>
       <c r="F41" t="n">
-        <v>99.9634177909</v>
+        <v>143.3638041798</v>
       </c>
       <c r="G41" t="inlineStr">
         <is>
@@ -1897,7 +1897,7 @@
         </is>
       </c>
       <c r="F42" t="n">
-        <v>24.34764605</v>
+        <v>35.6556382</v>
       </c>
       <c r="G42" t="inlineStr">
         <is>
@@ -1932,7 +1932,7 @@
         </is>
       </c>
       <c r="F43" t="n">
-        <v>23.398375</v>
+        <v>34.1355105</v>
       </c>
       <c r="G43" t="inlineStr">
         <is>
@@ -1967,7 +1967,7 @@
         </is>
       </c>
       <c r="F44" t="n">
-        <v>496.2506549</v>
+        <v>554.5128771</v>
       </c>
       <c r="G44" t="inlineStr">
         <is>
@@ -2037,7 +2037,7 @@
         </is>
       </c>
       <c r="F46" t="n">
-        <v>0.0014998431</v>
+        <v>0.002186249</v>
       </c>
       <c r="G46" t="inlineStr">
         <is>
@@ -2072,7 +2072,7 @@
         </is>
       </c>
       <c r="F47" t="n">
-        <v>35600.9745</v>
+        <v>43967.5873</v>
       </c>
       <c r="G47" t="inlineStr">
         <is>
@@ -2107,7 +2107,7 @@
         </is>
       </c>
       <c r="F48" t="n">
-        <v>0.0880971</v>
+        <v>0.1284192</v>
       </c>
       <c r="G48" t="inlineStr">
         <is>
@@ -2142,7 +2142,7 @@
         </is>
       </c>
       <c r="F49" t="n">
-        <v>126.2575857515</v>
+        <v>184.0327994096</v>
       </c>
       <c r="G49" t="inlineStr">
         <is>
@@ -2177,7 +2177,7 @@
         </is>
       </c>
       <c r="F50" t="n">
-        <v>78.16334437810001</v>
+        <v>112.5092303369</v>
       </c>
       <c r="G50" t="inlineStr">
         <is>
@@ -2212,7 +2212,7 @@
         </is>
       </c>
       <c r="F51" t="n">
-        <v>7.4889260672</v>
+        <v>10.9745258364</v>
       </c>
       <c r="G51" t="inlineStr">
         <is>
@@ -2247,7 +2247,7 @@
         </is>
       </c>
       <c r="F52" t="n">
-        <v>868.1485393352</v>
+        <v>1299.4072985544</v>
       </c>
       <c r="G52" t="inlineStr">
         <is>
@@ -2282,7 +2282,7 @@
         </is>
       </c>
       <c r="F53" t="n">
-        <v>27.84902393</v>
+        <v>42.00618968</v>
       </c>
       <c r="G53" t="inlineStr">
         <is>
@@ -2317,7 +2317,7 @@
         </is>
       </c>
       <c r="F54" t="n">
-        <v>60.9658879549</v>
+        <v>90.29868522220001</v>
       </c>
       <c r="G54" t="inlineStr">
         <is>
@@ -2352,7 +2352,7 @@
         </is>
       </c>
       <c r="F55" t="n">
-        <v>3.4697117</v>
+        <v>5.66510945</v>
       </c>
       <c r="G55" t="inlineStr">
         <is>
@@ -2387,7 +2387,7 @@
         </is>
       </c>
       <c r="F56" t="n">
-        <v>10066.6695389534</v>
+        <v>14779.4813678623</v>
       </c>
       <c r="G56" t="inlineStr">
         <is>
@@ -2422,7 +2422,7 @@
         </is>
       </c>
       <c r="F57" t="n">
-        <v>1.0899507375</v>
+        <v>1.7307645968</v>
       </c>
       <c r="G57" t="inlineStr">
         <is>
@@ -2457,7 +2457,7 @@
         </is>
       </c>
       <c r="F58" t="n">
-        <v>1.0745591334</v>
+        <v>1.7456761311</v>
       </c>
       <c r="G58" t="inlineStr">
         <is>
@@ -2492,7 +2492,7 @@
         </is>
       </c>
       <c r="F59" t="n">
-        <v>3473.2365710624</v>
+        <v>5172.8081389224</v>
       </c>
       <c r="G59" t="inlineStr">
         <is>
@@ -2527,7 +2527,7 @@
         </is>
       </c>
       <c r="F60" t="n">
-        <v>0.0370797067</v>
+        <v>0.0467458017</v>
       </c>
       <c r="G60" t="inlineStr">
         <is>
@@ -2562,7 +2562,7 @@
         </is>
       </c>
       <c r="F61" t="n">
-        <v>0.0001572051</v>
+        <v>0.0001637365</v>
       </c>
       <c r="G61" t="inlineStr">
         <is>
@@ -2597,7 +2597,7 @@
         </is>
       </c>
       <c r="F62" t="n">
-        <v>84.44345</v>
+        <v>89.70780000000001</v>
       </c>
       <c r="G62" t="inlineStr">
         <is>
@@ -2632,7 +2632,7 @@
         </is>
       </c>
       <c r="F63" t="n">
-        <v>171.2693766866</v>
+        <v>216.9448385559</v>
       </c>
       <c r="G63" t="inlineStr">
         <is>
@@ -2702,7 +2702,7 @@
         </is>
       </c>
       <c r="F65" t="n">
-        <v>0.0986944325</v>
+        <v>0.1456326816</v>
       </c>
       <c r="G65" t="inlineStr">
         <is>
@@ -2737,7 +2737,7 @@
         </is>
       </c>
       <c r="F66" t="n">
-        <v>233.4433500699</v>
+        <v>342.6837888172</v>
       </c>
       <c r="G66" t="inlineStr">
         <is>
@@ -2772,7 +2772,7 @@
         </is>
       </c>
       <c r="F67" t="n">
-        <v>195.1767777946</v>
+        <v>287.1938298594</v>
       </c>
       <c r="G67" t="inlineStr">
         <is>
@@ -2807,7 +2807,7 @@
         </is>
       </c>
       <c r="F68" t="n">
-        <v>68.041742654</v>
+        <v>123.0665639971</v>
       </c>
       <c r="G68" t="inlineStr">
         <is>
@@ -2842,7 +2842,7 @@
         </is>
       </c>
       <c r="F69" t="n">
-        <v>1.424332</v>
+        <v>1.6851835</v>
       </c>
       <c r="G69" t="inlineStr">
         <is>
@@ -2877,7 +2877,7 @@
         </is>
       </c>
       <c r="F70" t="n">
-        <v>28.3215987377</v>
+        <v>39.7414148545</v>
       </c>
       <c r="G70" t="inlineStr">
         <is>
@@ -2912,7 +2912,7 @@
         </is>
       </c>
       <c r="F71" t="n">
-        <v>71.5660516225</v>
+        <v>106.2695635308</v>
       </c>
       <c r="G71" t="inlineStr">
         <is>
@@ -2947,7 +2947,7 @@
         </is>
       </c>
       <c r="F72" t="n">
-        <v>1.4201915535</v>
+        <v>1.6851835666</v>
       </c>
       <c r="G72" t="inlineStr">
         <is>
@@ -2982,7 +2982,7 @@
         </is>
       </c>
       <c r="F73" t="n">
-        <v>114.1935810958</v>
+        <v>165.982710065</v>
       </c>
       <c r="G73" t="inlineStr">
         <is>
@@ -3017,7 +3017,7 @@
         </is>
       </c>
       <c r="F74" t="n">
-        <v>0.0228537523</v>
+        <v>0.0333139296</v>
       </c>
       <c r="G74" t="inlineStr">
         <is>
@@ -3052,7 +3052,7 @@
         </is>
       </c>
       <c r="F75" t="n">
-        <v>0.06950266500000001</v>
+        <v>0.10131408</v>
       </c>
       <c r="G75" t="inlineStr">
         <is>
@@ -3087,7 +3087,7 @@
         </is>
       </c>
       <c r="F76" t="n">
-        <v>0.2509693034</v>
+        <v>0.3658387488</v>
       </c>
       <c r="G76" t="inlineStr">
         <is>
@@ -3122,7 +3122,7 @@
         </is>
       </c>
       <c r="F77" t="n">
-        <v>517.8209328546</v>
+        <v>752.2626696477</v>
       </c>
       <c r="G77" t="inlineStr">
         <is>
@@ -3157,7 +3157,7 @@
         </is>
       </c>
       <c r="F78" t="n">
-        <v>12066.6509785139</v>
+        <v>14888.7210304649</v>
       </c>
       <c r="G78" t="inlineStr">
         <is>
@@ -3192,7 +3192,7 @@
         </is>
       </c>
       <c r="F79" t="n">
-        <v>182.94822</v>
+        <v>188.12976</v>
       </c>
       <c r="G79" t="inlineStr">
         <is>
@@ -3227,7 +3227,7 @@
         </is>
       </c>
       <c r="F80" t="n">
-        <v>4649.54854</v>
+        <v>6491.78894</v>
       </c>
       <c r="G80" t="inlineStr">
         <is>
@@ -3297,7 +3297,7 @@
         </is>
       </c>
       <c r="F82" t="n">
-        <v>3147.53439</v>
+        <v>4552.45973</v>
       </c>
       <c r="G82" t="inlineStr">
         <is>
@@ -3332,7 +3332,7 @@
         </is>
       </c>
       <c r="F83" t="n">
-        <v>256.76742</v>
+        <v>261.94896</v>
       </c>
       <c r="G83" t="inlineStr">
         <is>
@@ -3367,7 +3367,7 @@
         </is>
       </c>
       <c r="F84" t="n">
-        <v>22078.0617196826</v>
+        <v>31531.6541308297</v>
       </c>
       <c r="G84" t="inlineStr">
         <is>
@@ -3402,7 +3402,7 @@
         </is>
       </c>
       <c r="F85" t="n">
-        <v>0.4907499849</v>
+        <v>0.7279999776</v>
       </c>
       <c r="G85" t="inlineStr">
         <is>
@@ -3437,7 +3437,7 @@
         </is>
       </c>
       <c r="F86" t="n">
-        <v>18.8779537433</v>
+        <v>24.2424043086</v>
       </c>
       <c r="G86" t="inlineStr">
         <is>
@@ -3472,7 +3472,7 @@
         </is>
       </c>
       <c r="F87" t="n">
-        <v>707.2294144587</v>
+        <v>786.3975637238</v>
       </c>
       <c r="G87" t="inlineStr">
         <is>
@@ -3507,7 +3507,7 @@
         </is>
       </c>
       <c r="F88" t="n">
-        <v>0.4907499849</v>
+        <v>0.5636613253</v>
       </c>
       <c r="G88" t="inlineStr">
         <is>
@@ -3542,7 +3542,7 @@
         </is>
       </c>
       <c r="F89" t="n">
-        <v>12.2687499849</v>
+        <v>18.1999999776</v>
       </c>
       <c r="G89" t="inlineStr">
         <is>
@@ -3577,7 +3577,7 @@
         </is>
       </c>
       <c r="F90" t="n">
-        <v>912.8759326054</v>
+        <v>1345.5548408916</v>
       </c>
       <c r="G90" t="inlineStr">
         <is>
@@ -3612,7 +3612,7 @@
         </is>
       </c>
       <c r="F91" t="n">
-        <v>13.234859925</v>
+        <v>19.8938187557</v>
       </c>
       <c r="G91" t="inlineStr">
         <is>
@@ -3647,7 +3647,7 @@
         </is>
       </c>
       <c r="F92" t="n">
-        <v>4172.1726677679</v>
+        <v>6128.4011137286</v>
       </c>
       <c r="G92" t="inlineStr">
         <is>
@@ -3682,7 +3682,7 @@
         </is>
       </c>
       <c r="F93" t="n">
-        <v>343.2200002973</v>
+        <v>382.9107473286</v>
       </c>
       <c r="G93" t="inlineStr">
         <is>
@@ -3717,7 +3717,7 @@
         </is>
       </c>
       <c r="F94" t="n">
-        <v>21355.5253412426</v>
+        <v>29378.2215615146</v>
       </c>
       <c r="G94" t="inlineStr">
         <is>
@@ -3752,7 +3752,7 @@
         </is>
       </c>
       <c r="F95" t="n">
-        <v>2.109e-06</v>
+        <v>2.3349e-06</v>
       </c>
       <c r="G95" t="inlineStr">
         <is>
@@ -3787,7 +3787,7 @@
         </is>
       </c>
       <c r="F96" t="n">
-        <v>323.6956409823</v>
+        <v>351.1882615722</v>
       </c>
       <c r="G96" t="inlineStr">
         <is>
@@ -3822,7 +3822,7 @@
         </is>
       </c>
       <c r="F97" t="n">
-        <v>160.7424</v>
+        <v>199.7245674278</v>
       </c>
       <c r="G97" t="inlineStr">
         <is>
@@ -3857,7 +3857,7 @@
         </is>
       </c>
       <c r="F98" t="n">
-        <v>4864.6088185825</v>
+        <v>7119.6599133504</v>
       </c>
       <c r="G98" t="inlineStr">
         <is>
@@ -3892,7 +3892,7 @@
         </is>
       </c>
       <c r="F99" t="n">
-        <v>756.2233465401</v>
+        <v>793.8196577797</v>
       </c>
       <c r="G99" t="inlineStr">
         <is>
@@ -3927,7 +3927,7 @@
         </is>
       </c>
       <c r="F100" t="n">
-        <v>53250.015698637</v>
+        <v>76793.3337620845</v>
       </c>
       <c r="G100" t="inlineStr">
         <is>
@@ -3962,7 +3962,7 @@
         </is>
       </c>
       <c r="F101" t="n">
-        <v>312.2180085215</v>
+        <v>319.4971400577</v>
       </c>
       <c r="G101" t="inlineStr">
         <is>
@@ -3997,7 +3997,7 @@
         </is>
       </c>
       <c r="F102" t="n">
-        <v>5714.1329628324</v>
+        <v>8191.4321541478</v>
       </c>
       <c r="G102" t="inlineStr">
         <is>
@@ -4032,7 +4032,7 @@
         </is>
       </c>
       <c r="F103" t="n">
-        <v>572.4725372717</v>
+        <v>834.589719067</v>
       </c>
       <c r="G103" t="inlineStr">
         <is>
@@ -4067,7 +4067,7 @@
         </is>
       </c>
       <c r="F104" t="n">
-        <v>366.6316266741</v>
+        <v>539.4406266741</v>
       </c>
       <c r="G104" t="inlineStr">
         <is>
@@ -4102,7 +4102,7 @@
         </is>
       </c>
       <c r="F105" t="n">
-        <v>377.559</v>
+        <v>550.3680000000001</v>
       </c>
       <c r="G105" t="inlineStr">
         <is>
@@ -4137,7 +4137,7 @@
         </is>
       </c>
       <c r="F106" t="n">
-        <v>852.0738010447</v>
+        <v>910.4767480777</v>
       </c>
       <c r="G106" t="inlineStr">
         <is>
@@ -4277,7 +4277,7 @@
         </is>
       </c>
       <c r="F110" t="n">
-        <v>5208.8544333595</v>
+        <v>7486.0071845132</v>
       </c>
       <c r="G110" t="inlineStr">
         <is>
@@ -4312,7 +4312,7 @@
         </is>
       </c>
       <c r="F111" t="n">
-        <v>9.4397587632</v>
+        <v>12.6955212721</v>
       </c>
       <c r="G111" t="inlineStr">
         <is>
@@ -4347,7 +4347,7 @@
         </is>
       </c>
       <c r="F112" t="n">
-        <v>13.9495974567</v>
+        <v>19.7037296251</v>
       </c>
       <c r="G112" t="inlineStr">
         <is>
@@ -4382,7 +4382,7 @@
         </is>
       </c>
       <c r="F113" t="n">
-        <v>47.3195803431</v>
+        <v>53.0430548856</v>
       </c>
       <c r="G113" t="inlineStr">
         <is>
@@ -4417,7 +4417,7 @@
         </is>
       </c>
       <c r="F114" t="n">
-        <v>160.678752495</v>
+        <v>237.4633765258</v>
       </c>
       <c r="G114" t="inlineStr">
         <is>
@@ -4452,7 +4452,7 @@
         </is>
       </c>
       <c r="F115" t="n">
-        <v>53.4203274625</v>
+        <v>67.0674566494</v>
       </c>
       <c r="G115" t="inlineStr">
         <is>
@@ -4487,7 +4487,7 @@
         </is>
       </c>
       <c r="F116" t="n">
-        <v>1314.0229964301</v>
+        <v>1915.747542436</v>
       </c>
       <c r="G116" t="inlineStr">
         <is>
@@ -4522,7 +4522,7 @@
         </is>
       </c>
       <c r="F117" t="n">
-        <v>9.438974999999999</v>
+        <v>9.766575</v>
       </c>
       <c r="G117" t="inlineStr">
         <is>
@@ -4557,7 +4557,7 @@
         </is>
       </c>
       <c r="F118" t="n">
-        <v>10.5926806058</v>
+        <v>14.2863263381</v>
       </c>
       <c r="G118" t="inlineStr">
         <is>
@@ -4592,7 +4592,7 @@
         </is>
       </c>
       <c r="F119" t="n">
-        <v>62.8841987549</v>
+        <v>68.92682186490001</v>
       </c>
       <c r="G119" t="inlineStr">
         <is>
@@ -4627,7 +4627,7 @@
         </is>
       </c>
       <c r="F120" t="n">
-        <v>1.593632331</v>
+        <v>2.3485122416</v>
       </c>
       <c r="G120" t="inlineStr">
         <is>
@@ -4662,7 +4662,7 @@
         </is>
       </c>
       <c r="F121" t="n">
-        <v>2675.6432846923</v>
+        <v>3656.6380280844</v>
       </c>
       <c r="G121" t="inlineStr">
         <is>
@@ -4697,7 +4697,7 @@
         </is>
       </c>
       <c r="F122" t="n">
-        <v>7.7805</v>
+        <v>12.1485</v>
       </c>
       <c r="G122" t="inlineStr">
         <is>
@@ -4732,7 +4732,7 @@
         </is>
       </c>
       <c r="F123" t="n">
-        <v>75.69373774739999</v>
+        <v>110.3633213639</v>
       </c>
       <c r="G123" t="inlineStr">
         <is>
@@ -4802,7 +4802,7 @@
         </is>
       </c>
       <c r="F125" t="n">
-        <v>5.7901784147</v>
+        <v>8.4570259233</v>
       </c>
       <c r="G125" t="inlineStr">
         <is>
@@ -4837,7 +4837,7 @@
         </is>
       </c>
       <c r="F126" t="n">
-        <v>0.00088816</v>
+        <v>0.00133224</v>
       </c>
       <c r="G126" t="inlineStr">
         <is>
@@ -4872,7 +4872,7 @@
         </is>
       </c>
       <c r="F127" t="n">
-        <v>37.7840855443</v>
+        <v>55.0833312935</v>
       </c>
       <c r="G127" t="inlineStr">
         <is>
@@ -4907,7 +4907,7 @@
         </is>
       </c>
       <c r="F128" t="n">
-        <v>133.9115030289</v>
+        <v>195.2637385121</v>
       </c>
       <c r="G128" t="inlineStr">
         <is>
@@ -4942,7 +4942,7 @@
         </is>
       </c>
       <c r="F129" t="n">
-        <v>133.2502781539</v>
+        <v>194.260273295</v>
       </c>
       <c r="G129" t="inlineStr">
         <is>
@@ -4977,7 +4977,7 @@
         </is>
       </c>
       <c r="F130" t="n">
-        <v>1.421238</v>
+        <v>2.094456</v>
       </c>
       <c r="G130" t="inlineStr">
         <is>
@@ -5082,7 +5082,7 @@
         </is>
       </c>
       <c r="F133" t="n">
-        <v>83.2609673489</v>
+        <v>117.1548116507</v>
       </c>
       <c r="G133" t="inlineStr">
         <is>
@@ -5117,7 +5117,7 @@
         </is>
       </c>
       <c r="F134" t="n">
-        <v>116.276186</v>
+        <v>169.495872</v>
       </c>
       <c r="G134" t="inlineStr">
         <is>
@@ -5152,7 +5152,7 @@
         </is>
       </c>
       <c r="F135" t="n">
-        <v>4485.8566436044</v>
+        <v>6851.7385017163</v>
       </c>
       <c r="G135" t="inlineStr">
         <is>
@@ -5187,7 +5187,7 @@
         </is>
       </c>
       <c r="F136" t="n">
-        <v>1147.4491423515</v>
+        <v>1907.8087423515</v>
       </c>
       <c r="G136" t="inlineStr">
         <is>
@@ -5222,7 +5222,7 @@
         </is>
       </c>
       <c r="F137" t="n">
-        <v>1660.04985548</v>
+        <v>2420.40945548</v>
       </c>
       <c r="G137" t="inlineStr">
         <is>
@@ -5257,7 +5257,7 @@
         </is>
       </c>
       <c r="F138" t="n">
-        <v>2.9597507463</v>
+        <v>4.3989038685</v>
       </c>
       <c r="G138" t="inlineStr">
         <is>
@@ -5292,7 +5292,7 @@
         </is>
       </c>
       <c r="F139" t="n">
-        <v>1286.3331333505</v>
+        <v>1737.5870521821</v>
       </c>
       <c r="G139" t="inlineStr">
         <is>
@@ -5327,7 +5327,7 @@
         </is>
       </c>
       <c r="F140" t="n">
-        <v>7189.9062170882</v>
+        <v>10357.6545186181</v>
       </c>
       <c r="G140" t="inlineStr">
         <is>
@@ -5362,7 +5362,7 @@
         </is>
       </c>
       <c r="F141" t="n">
-        <v>21281.5932880336</v>
+        <v>29758.798985453</v>
       </c>
       <c r="G141" t="inlineStr">
         <is>
@@ -5397,7 +5397,7 @@
         </is>
       </c>
       <c r="F142" t="n">
-        <v>71.3720864754</v>
+        <v>104.0393199114</v>
       </c>
       <c r="G142" t="inlineStr">
         <is>
@@ -5432,7 +5432,7 @@
         </is>
       </c>
       <c r="F143" t="n">
-        <v>1379.1889799141</v>
+        <v>1963.2218029324</v>
       </c>
       <c r="G143" t="inlineStr">
         <is>
@@ -5467,7 +5467,7 @@
         </is>
       </c>
       <c r="F144" t="n">
-        <v>22.8571359778</v>
+        <v>39.7633114887</v>
       </c>
       <c r="G144" t="inlineStr">
         <is>
@@ -5502,7 +5502,7 @@
         </is>
       </c>
       <c r="F145" t="n">
-        <v>771.9926668418</v>
+        <v>881.3063252442</v>
       </c>
       <c r="G145" t="inlineStr">
         <is>
@@ -5572,7 +5572,7 @@
         </is>
       </c>
       <c r="F147" t="n">
-        <v>53177.084449512</v>
+        <v>71161.0831991483</v>
       </c>
       <c r="G147" t="inlineStr">
         <is>
@@ -5607,7 +5607,7 @@
         </is>
       </c>
       <c r="F148" t="n">
-        <v>0.0010741474</v>
+        <v>0.0015760416</v>
       </c>
       <c r="G148" t="inlineStr">
         <is>
@@ -5642,7 +5642,7 @@
         </is>
       </c>
       <c r="F149" t="n">
-        <v>1914.9600314418</v>
+        <v>2530.8257425658</v>
       </c>
       <c r="G149" t="inlineStr">
         <is>
@@ -5677,7 +5677,7 @@
         </is>
       </c>
       <c r="F150" t="n">
-        <v>86.787900146</v>
+        <v>89.150122475</v>
       </c>
       <c r="G150" t="inlineStr">
         <is>
@@ -5712,7 +5712,7 @@
         </is>
       </c>
       <c r="F151" t="n">
-        <v>9347.2149325635</v>
+        <v>11968.7550562134</v>
       </c>
       <c r="G151" t="inlineStr">
         <is>
@@ -5747,7 +5747,7 @@
         </is>
       </c>
       <c r="F152" t="n">
-        <v>148.5581334661</v>
+        <v>179.1275690148</v>
       </c>
       <c r="G152" t="inlineStr">
         <is>
@@ -5782,7 +5782,7 @@
         </is>
       </c>
       <c r="F153" t="n">
-        <v>1104.0924220489</v>
+        <v>1494.5911312298</v>
       </c>
       <c r="G153" t="inlineStr">
         <is>
@@ -5817,7 +5817,7 @@
         </is>
       </c>
       <c r="F154" t="n">
-        <v>0.157312246</v>
+        <v>0.177546642</v>
       </c>
       <c r="G154" t="inlineStr">
         <is>
@@ -5957,7 +5957,7 @@
         </is>
       </c>
       <c r="F158" t="n">
-        <v>0.455097552</v>
+        <v>0.455119392</v>
       </c>
       <c r="G158" t="inlineStr">
         <is>
@@ -5992,7 +5992,7 @@
         </is>
       </c>
       <c r="F159" t="n">
-        <v>11.546665858</v>
+        <v>12.58948873</v>
       </c>
       <c r="G159" t="inlineStr">
         <is>
@@ -6027,7 +6027,7 @@
         </is>
       </c>
       <c r="F160" t="n">
-        <v>11.846281902</v>
+        <v>14.510554058</v>
       </c>
       <c r="G160" t="inlineStr">
         <is>
@@ -6062,7 +6062,7 @@
         </is>
       </c>
       <c r="F161" t="n">
-        <v>0.09107225400000001</v>
+        <v>0.09108918000000001</v>
       </c>
       <c r="G161" t="inlineStr">
         <is>
@@ -6097,7 +6097,7 @@
         </is>
       </c>
       <c r="F162" t="n">
-        <v>0.091022204</v>
+        <v>0.091028756</v>
       </c>
       <c r="G162" t="inlineStr">
         <is>
@@ -6167,7 +6167,7 @@
         </is>
       </c>
       <c r="F164" t="n">
-        <v>2626.989432189</v>
+        <v>3955.661311808</v>
       </c>
       <c r="G164" t="inlineStr">
         <is>
@@ -6202,7 +6202,7 @@
         </is>
       </c>
       <c r="F165" t="n">
-        <v>9.128752221699999</v>
+        <v>12.5447968058</v>
       </c>
       <c r="G165" t="inlineStr">
         <is>
@@ -6237,7 +6237,7 @@
         </is>
       </c>
       <c r="F166" t="n">
-        <v>16.0037708058</v>
+        <v>21.7872895452</v>
       </c>
       <c r="G166" t="inlineStr">
         <is>
@@ -6272,7 +6272,7 @@
         </is>
       </c>
       <c r="F167" t="n">
-        <v>0.0038460557</v>
+        <v>0.0059024252</v>
       </c>
       <c r="G167" t="inlineStr">
         <is>
@@ -6307,7 +6307,7 @@
         </is>
       </c>
       <c r="F168" t="n">
-        <v>6.916e-05</v>
+        <v>9.282e-05</v>
       </c>
       <c r="G168" t="inlineStr">
         <is>
@@ -6342,7 +6342,7 @@
         </is>
       </c>
       <c r="F169" t="n">
-        <v>0.000662025</v>
+        <v>0.00096915</v>
       </c>
       <c r="G169" t="inlineStr">
         <is>
@@ -6377,7 +6377,7 @@
         </is>
       </c>
       <c r="F170" t="n">
-        <v>3.5035e-05</v>
+        <v>5.187e-05</v>
       </c>
       <c r="G170" t="inlineStr">
         <is>
@@ -6412,7 +6412,7 @@
         </is>
       </c>
       <c r="F171" t="n">
-        <v>24.590330339</v>
+        <v>34.872477217</v>
       </c>
       <c r="G171" t="inlineStr">
         <is>
@@ -6447,7 +6447,7 @@
         </is>
       </c>
       <c r="F172" t="n">
-        <v>7.462e-05</v>
+        <v>0.000107744</v>
       </c>
       <c r="G172" t="inlineStr">
         <is>
@@ -6482,7 +6482,7 @@
         </is>
       </c>
       <c r="F173" t="n">
-        <v>0.6547884094999999</v>
+        <v>0.9525613643</v>
       </c>
       <c r="G173" t="inlineStr">
         <is>
@@ -6517,7 +6517,7 @@
         </is>
       </c>
       <c r="F174" t="n">
-        <v>0.9047634666</v>
+        <v>1.3185857326</v>
       </c>
       <c r="G174" t="inlineStr">
         <is>
@@ -6552,7 +6552,7 @@
         </is>
       </c>
       <c r="F175" t="n">
-        <v>29397.8149025704</v>
+        <v>40962.7431490213</v>
       </c>
       <c r="G175" t="inlineStr">
         <is>
@@ -6587,7 +6587,7 @@
         </is>
       </c>
       <c r="F176" t="n">
-        <v>0.0442590753</v>
+        <v>0.06666566559999999</v>
       </c>
       <c r="G176" t="inlineStr">
         <is>
@@ -6622,7 +6622,7 @@
         </is>
       </c>
       <c r="F177" t="n">
-        <v>0.0005246881</v>
+        <v>0.0007762044</v>
       </c>
       <c r="G177" t="inlineStr">
         <is>
@@ -6657,7 +6657,7 @@
         </is>
       </c>
       <c r="F178" t="n">
-        <v>0.0512264277</v>
+        <v>0.0749601471</v>
       </c>
       <c r="G178" t="inlineStr">
         <is>
@@ -6692,7 +6692,7 @@
         </is>
       </c>
       <c r="F179" t="n">
-        <v>5.930493209</v>
+        <v>7.8737505948</v>
       </c>
       <c r="G179" t="inlineStr">
         <is>
@@ -6727,7 +6727,7 @@
         </is>
       </c>
       <c r="F180" t="n">
-        <v>0.0005747077</v>
+        <v>0.0008345234999999999</v>
       </c>
       <c r="G180" t="inlineStr">
         <is>
@@ -6762,7 +6762,7 @@
         </is>
       </c>
       <c r="F181" t="n">
-        <v>0.0016330453</v>
+        <v>0.0023665348</v>
       </c>
       <c r="G181" t="inlineStr">
         <is>
@@ -6797,7 +6797,7 @@
         </is>
       </c>
       <c r="F182" t="n">
-        <v>14.0911359525</v>
+        <v>20.6345898337</v>
       </c>
       <c r="G182" t="inlineStr">
         <is>
@@ -6832,7 +6832,7 @@
         </is>
       </c>
       <c r="F183" t="n">
-        <v>0.0567836938</v>
+        <v>0.0836976546</v>
       </c>
       <c r="G183" t="inlineStr">
         <is>
@@ -6867,7 +6867,7 @@
         </is>
       </c>
       <c r="F184" t="n">
-        <v>1411.4715951225</v>
+        <v>1902.1013961296</v>
       </c>
       <c r="G184" t="inlineStr">
         <is>
@@ -6902,7 +6902,7 @@
         </is>
       </c>
       <c r="F185" t="n">
-        <v>1.7899800062</v>
+        <v>2.8790802163</v>
       </c>
       <c r="G185" t="inlineStr">
         <is>
@@ -6937,7 +6937,7 @@
         </is>
       </c>
       <c r="F186" t="n">
-        <v>11073.5401686086</v>
+        <v>16399.0091283711</v>
       </c>
       <c r="G186" t="inlineStr">
         <is>
@@ -6972,7 +6972,7 @@
         </is>
       </c>
       <c r="F187" t="n">
-        <v>0.0005881497</v>
+        <v>0.0008454655</v>
       </c>
       <c r="G187" t="inlineStr">
         <is>
@@ -7007,7 +7007,7 @@
         </is>
       </c>
       <c r="F188" t="n">
-        <v>0.0032658275</v>
+        <v>0.0042247144</v>
       </c>
       <c r="G188" t="inlineStr">
         <is>
@@ -7042,7 +7042,7 @@
         </is>
       </c>
       <c r="F189" t="n">
-        <v>6.855e-07</v>
+        <v>9.855999999999999e-07</v>
       </c>
       <c r="G189" t="inlineStr">
         <is>
@@ -7077,7 +7077,7 @@
         </is>
       </c>
       <c r="F190" t="n">
-        <v>8.073e-06</v>
+        <v>1.1592e-05</v>
       </c>
       <c r="G190" t="inlineStr">
         <is>
@@ -7112,7 +7112,7 @@
         </is>
       </c>
       <c r="F191" t="n">
-        <v>7573.0797291726</v>
+        <v>10717.7302611493</v>
       </c>
       <c r="G191" t="inlineStr">
         <is>
@@ -7147,11 +7147,11 @@
         </is>
       </c>
       <c r="F192" t="n">
-        <v>2.09755</v>
+        <v>0.0001908498</v>
       </c>
       <c r="G192" t="inlineStr">
         <is>
-          <t>Environment$dev</t>
+          <t>Environment$common</t>
         </is>
       </c>
     </row>
@@ -7182,11 +7182,11 @@
         </is>
       </c>
       <c r="F193" t="n">
-        <v>62.972</v>
+        <v>2.9547219746</v>
       </c>
       <c r="G193" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$dev</t>
         </is>
       </c>
     </row>
@@ -7217,11 +7217,11 @@
         </is>
       </c>
       <c r="F194" t="n">
-        <v>2.09755</v>
+        <v>91.819</v>
       </c>
       <c r="G194" t="inlineStr">
         <is>
-          <t>Environment$ops</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -7252,11 +7252,11 @@
         </is>
       </c>
       <c r="F195" t="n">
-        <v>90.1814938591</v>
+        <v>2.8309821949</v>
       </c>
       <c r="G195" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$ops</t>
         </is>
       </c>
     </row>
@@ -7287,11 +7287,11 @@
         </is>
       </c>
       <c r="F196" t="n">
-        <v>56.9613993298</v>
+        <v>0.4570083199</v>
       </c>
       <c r="G196" t="inlineStr">
         <is>
-          <t>Environment$shared</t>
+          <t>Environment$prd</t>
         </is>
       </c>
     </row>
@@ -7322,11 +7322,11 @@
         </is>
       </c>
       <c r="F197" t="n">
-        <v>4.18145</v>
+        <v>130.8371912307</v>
       </c>
       <c r="G197" t="inlineStr">
         <is>
-          <t>Environment$stg</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -7353,15 +7353,15 @@
       </c>
       <c r="E198" t="inlineStr">
         <is>
-          <t>Amazon WorkSpaces</t>
+          <t>Amazon Virtual Private Cloud</t>
         </is>
       </c>
       <c r="F198" t="n">
-        <v>216.2887999326</v>
+        <v>83.0991114342</v>
       </c>
       <c r="G198" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$shared</t>
         </is>
       </c>
     </row>
@@ -7388,15 +7388,15 @@
       </c>
       <c r="E199" t="inlineStr">
         <is>
-          <t>AmazonCloudWatch</t>
+          <t>Amazon Virtual Private Cloud</t>
         </is>
       </c>
       <c r="F199" t="n">
-        <v>9703.735095814</v>
+        <v>5.1135314001</v>
       </c>
       <c r="G199" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$stg</t>
         </is>
       </c>
     </row>
@@ -7423,15 +7423,15 @@
       </c>
       <c r="E200" t="inlineStr">
         <is>
-          <t>AmazonCloudWatch</t>
+          <t>Amazon WorkSpaces</t>
         </is>
       </c>
       <c r="F200" t="n">
-        <v>1.43771875</v>
+        <v>218.2998999326</v>
       </c>
       <c r="G200" t="inlineStr">
         <is>
-          <t>Environment$dev</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -7462,11 +7462,11 @@
         </is>
       </c>
       <c r="F201" t="n">
-        <v>1.4885</v>
+        <v>13077.0862210177</v>
       </c>
       <c r="G201" t="inlineStr">
         <is>
-          <t>Environment$management</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -7497,11 +7497,11 @@
         </is>
       </c>
       <c r="F202" t="n">
-        <v>572.8042982898</v>
+        <v>1.5429375</v>
       </c>
       <c r="G202" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$dev</t>
         </is>
       </c>
     </row>
@@ -7532,11 +7532,11 @@
         </is>
       </c>
       <c r="F203" t="n">
-        <v>2591.1368593169</v>
+        <v>1.86103125</v>
       </c>
       <c r="G203" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$management</t>
         </is>
       </c>
     </row>
@@ -7563,15 +7563,15 @@
       </c>
       <c r="E204" t="inlineStr">
         <is>
-          <t>AmazonWorkMail</t>
+          <t>AmazonCloudWatch</t>
         </is>
       </c>
       <c r="F204" t="n">
-        <v>122.3570832104</v>
+        <v>836.1506065505999</v>
       </c>
       <c r="G204" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -7598,15 +7598,15 @@
       </c>
       <c r="E205" t="inlineStr">
         <is>
-          <t>Aviatrix Secure Networking Platform Metered - 24x7 Support with Copilot</t>
+          <t>AmazonCloudWatch</t>
         </is>
       </c>
       <c r="F205" t="n">
-        <v>0.9</v>
+        <v>3831.9700555904</v>
       </c>
       <c r="G205" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -7633,11 +7633,11 @@
       </c>
       <c r="E206" t="inlineStr">
         <is>
-          <t>CloudWatch Events</t>
+          <t>AmazonWorkMail</t>
         </is>
       </c>
       <c r="F206" t="n">
-        <v>1.5568427774</v>
+        <v>178.3599998208</v>
       </c>
       <c r="G206" t="inlineStr">
         <is>
@@ -7668,11 +7668,11 @@
       </c>
       <c r="E207" t="inlineStr">
         <is>
-          <t>Savings Plans for AWS Compute usage</t>
+          <t>Aviatrix Secure Networking Platform Metered - 24x7 Support with Copilot</t>
         </is>
       </c>
       <c r="F207" t="n">
-        <v>16780.8</v>
+        <v>0.9</v>
       </c>
       <c r="G207" t="inlineStr">
         <is>
@@ -7703,11 +7703,11 @@
       </c>
       <c r="E208" t="inlineStr">
         <is>
-          <t>Tax</t>
+          <t>CloudWatch Events</t>
         </is>
       </c>
       <c r="F208" t="n">
-        <v>7193.53</v>
+        <v>1.9097642063</v>
       </c>
       <c r="G208" t="inlineStr">
         <is>
@@ -7738,13 +7738,83 @@
       </c>
       <c r="E209" t="inlineStr">
         <is>
+          <t>Savings Plans for AWS Compute usage</t>
+        </is>
+      </c>
+      <c r="F209" t="n">
+        <v>16780.8</v>
+      </c>
+      <c r="G209" t="inlineStr">
+        <is>
+          <t>Environment$</t>
+        </is>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="inlineStr">
+        <is>
+          <t>FEB</t>
+        </is>
+      </c>
+      <c r="B210" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="C210" t="inlineStr">
+        <is>
+          <t>Entercom Communications</t>
+        </is>
+      </c>
+      <c r="D210" t="inlineStr">
+        <is>
+          <t>724972922289</t>
+        </is>
+      </c>
+      <c r="E210" t="inlineStr">
+        <is>
+          <t>Tax</t>
+        </is>
+      </c>
+      <c r="F210" t="n">
+        <v>9946.299999999999</v>
+      </c>
+      <c r="G210" t="inlineStr">
+        <is>
+          <t>Environment$</t>
+        </is>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="inlineStr">
+        <is>
+          <t>FEB</t>
+        </is>
+      </c>
+      <c r="B211" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="C211" t="inlineStr">
+        <is>
+          <t>Entercom Communications</t>
+        </is>
+      </c>
+      <c r="D211" t="inlineStr">
+        <is>
+          <t>724972922289</t>
+        </is>
+      </c>
+      <c r="E211" t="inlineStr">
+        <is>
           <t>dbt Cloud Enterprise</t>
         </is>
       </c>
-      <c r="F209" t="n">
+      <c r="F211" t="n">
         <v>9687.5</v>
       </c>
-      <c r="G209" t="inlineStr">
+      <c r="G211" t="inlineStr">
         <is>
           <t>Environment$</t>
         </is>

</xml_diff>